<commit_message>
task 3 - Array Methods done
</commit_message>
<xml_diff>
--- a/MATH 108X/GroupAssignment - W03.xlsx
+++ b/MATH 108X/GroupAssignment - W03.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\Desktop\Leti\Programming\MATH 108X\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1184AF03-41EA-4D8C-9B1D-8441C75F1CE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4AFA1DB-808F-40C5-8576-95B196072054}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="500" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Step 1" sheetId="1" r:id="rId1"/>
@@ -20,16 +20,8 @@
     <sheet name="Step 5" sheetId="7" r:id="rId5"/>
     <sheet name="Step 6 " sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="181029"/>
   <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -38,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
   <si>
     <t>Quantitative Reasoning Process</t>
   </si>
@@ -127,6 +119,9 @@
   </si>
   <si>
     <t>Notice that Juan didn't follow-through with the informed decision he made previously.  Which type of logical fallacy does this example represent? Explain.</t>
+  </si>
+  <si>
+    <t>{</t>
   </si>
 </sst>
 </file>
@@ -1452,6 +1447,12 @@
             <a:rPr lang="en-US" sz="1800" baseline="0"/>
             <a:t>Money saved.</a:t>
           </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" baseline="0"/>
+            <a:t>How much is willing to borrow.</a:t>
+          </a:r>
           <a:endParaRPr lang="en-US" sz="1800"/>
         </a:p>
       </xdr:txBody>
@@ -1516,6 +1517,23 @@
           </a:r>
         </a:p>
         <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800"/>
+            <a:t>Maybe Sara</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" baseline="0"/>
+            <a:t> still want to marry.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" baseline="0"/>
+            <a:t>They won't break up.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1800"/>
+        </a:p>
+        <a:p>
           <a:endParaRPr lang="en-US" sz="1800"/>
         </a:p>
       </xdr:txBody>
@@ -1574,15 +1592,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>678428</xdr:colOff>
+      <xdr:colOff>739388</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>38101</xdr:rowOff>
+      <xdr:rowOff>53341</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>598291</xdr:colOff>
+      <xdr:colOff>659251</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>368300</xdr:rowOff>
+      <xdr:rowOff>383540</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1605,8 +1623,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3586728" y="609601"/>
-          <a:ext cx="3221863" cy="2819399"/>
+          <a:off x="5334248" y="1645921"/>
+          <a:ext cx="3242183" cy="2806699"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1723,10 +1741,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>1362075</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>53340</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>144780</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1741,8 +1759,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5419725" y="5000625"/>
-          <a:ext cx="4676775" cy="1666875"/>
+          <a:off x="5425440" y="4991100"/>
+          <a:ext cx="4747260" cy="1798320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1769,26 +1787,49 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1800"/>
-            <a:t>1.</a:t>
+            <a:t>1.White</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" baseline="0"/>
+            <a:t> gold plain setting with a</a:t>
           </a:r>
         </a:p>
         <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" baseline="0"/>
+            <a:t>   Diamond 1/4 carat</a:t>
+          </a:r>
           <a:endParaRPr lang="en-US" sz="1800"/>
         </a:p>
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1800"/>
-            <a:t>2.</a:t>
+            <a:t>2.Total cost:</a:t>
           </a:r>
-        </a:p>
-        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" baseline="0"/>
+            <a:t> $500 + $400 = $900 He doesn't need to borrow</a:t>
+          </a:r>
           <a:endParaRPr lang="en-US" sz="1800"/>
         </a:p>
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1800"/>
-            <a:t>3.</a:t>
+            <a:t>3.$1150</a:t>
           </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" baseline="0"/>
+            <a:t> - $900 = $250 He doesn't need to pay beyond his savings</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" baseline="0"/>
+            <a:t>   </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1800"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -2074,11 +2115,11 @@
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1800" baseline="0"/>
-            <a:t> </a:t>
+            <a:t> T</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1800"/>
-            <a:t>the seller emotionally manipulated Juan by making him think about how happy Sara would be with a more expensive ring, with the purpose of earning more money, and not because it is the best financial option for Juan.</a:t>
+            <a:t>he seller emotionally manipulated Juan by making him think about how happy Sara would be with a more expensive ring, with the purpose of earning more money, and not because it is the best financial option for Juan.</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -2194,8 +2235,15 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1800"/>
-            <a:t>Because they use the fallacy "Appeal to emotion" a lot and most of the time emotions win over logic.</a:t>
+            <a:t>Because they use the fallacy "Appeal to emotion" a lot and most of the time emotions win over logic. Sometimes emotions can blur your</a:t>
           </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" baseline="0"/>
+            <a:t> mind. Marketing makes you want to be instantly gratified.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1800"/>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -2253,6 +2301,14 @@
         <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
         <a:lstStyle/>
         <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800"/>
+            <a:t>You need</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1800" baseline="0"/>
+            <a:t> to regulate your emotions and think if you really need it before you act.</a:t>
+          </a:r>
           <a:endParaRPr lang="en-US" sz="1800"/>
         </a:p>
       </xdr:txBody>
@@ -2527,8 +2583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B1:R35"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="L24" sqref="L24"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="L25" sqref="L25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8984375" defaultRowHeight="15.6"/>
@@ -2990,7 +3046,9 @@
       <c r="I24" s="1"/>
       <c r="J24" s="1"/>
       <c r="K24" s="12"/>
-      <c r="L24" s="16"/>
+      <c r="L24" s="16" t="s">
+        <v>24</v>
+      </c>
       <c r="M24" s="12"/>
       <c r="N24" s="8"/>
       <c r="O24" s="8"/>
@@ -3872,8 +3930,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B2:Q35"/>
   <sheetViews>
-    <sheetView topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8984375" defaultRowHeight="15.6"/>
@@ -4505,8 +4563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B2:O38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16:N20"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8984375" defaultRowHeight="15.6"/>
@@ -5139,7 +5197,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="B2:P37"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>

</xml_diff>